<commit_message>
Updated all the files - added new versions
</commit_message>
<xml_diff>
--- a/Gantt Chartv1.xlsx
+++ b/Gantt Chartv1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashwin\Desktop\CYCLONE\Electronics - GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahuja\Desktop\CanSat\Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Week Commencing:</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Mar</t>
+  </si>
+  <si>
+    <t>Data Analysis</t>
   </si>
 </sst>
 </file>
@@ -243,12 +246,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -256,6 +253,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF92D050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkVertical">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF92D050"/>
       </patternFill>
     </fill>
@@ -287,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -300,7 +303,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -313,16 +315,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,11 +607,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y46"/>
+  <dimension ref="A1:Y47"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="82" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z42" sqref="Z42"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A9" zoomScale="82" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:Y47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -620,114 +624,114 @@
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19" t="s">
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19" t="s">
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19" t="s">
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19" t="s">
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="15">
         <v>19</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="15">
         <v>26</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="16">
         <v>2</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="16">
         <v>9</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="16">
         <v>16</v>
       </c>
-      <c r="H2" s="17">
+      <c r="H2" s="16">
         <v>23</v>
       </c>
-      <c r="I2" s="17">
+      <c r="I2" s="16">
         <v>30</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="16">
         <v>7</v>
       </c>
-      <c r="K2" s="17">
+      <c r="K2" s="16">
         <v>14</v>
       </c>
-      <c r="L2" s="17">
+      <c r="L2" s="16">
         <v>21</v>
       </c>
-      <c r="M2" s="17">
+      <c r="M2" s="16">
         <v>28</v>
       </c>
-      <c r="N2" s="17">
+      <c r="N2" s="16">
         <v>4</v>
       </c>
-      <c r="O2" s="17">
+      <c r="O2" s="16">
         <v>11</v>
       </c>
-      <c r="P2" s="17">
+      <c r="P2" s="16">
         <v>18</v>
       </c>
-      <c r="Q2" s="17">
+      <c r="Q2" s="16">
         <v>25</v>
       </c>
-      <c r="R2" s="17">
+      <c r="R2" s="16">
         <v>1</v>
       </c>
-      <c r="S2" s="17">
+      <c r="S2" s="16">
         <v>8</v>
       </c>
-      <c r="T2" s="17">
+      <c r="T2" s="16">
         <v>15</v>
       </c>
-      <c r="U2" s="17">
+      <c r="U2" s="16">
         <v>22</v>
       </c>
-      <c r="V2" s="17">
+      <c r="V2" s="16">
         <v>29</v>
       </c>
-      <c r="W2" s="18">
+      <c r="W2" s="17">
         <v>7</v>
       </c>
-      <c r="X2" s="17">
+      <c r="X2" s="16">
         <v>14</v>
       </c>
-      <c r="Y2" s="17">
+      <c r="Y2" s="16">
         <v>21</v>
       </c>
     </row>
@@ -772,11 +776,11 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
@@ -796,23 +800,23 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
@@ -826,17 +830,17 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
@@ -855,7 +859,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="13"/>
+      <c r="F7" s="12"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -865,10 +869,10 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
@@ -886,22 +890,22 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="6"/>
+      <c r="Q8" s="12"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
     </row>
@@ -993,15 +997,15 @@
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
@@ -1025,9 +1029,9 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -1056,18 +1060,18 @@
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
       <c r="M14" s="11"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
       <c r="T14" s="8"/>
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
@@ -1077,100 +1081,102 @@
     </row>
     <row r="15" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
+      <c r="B15" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="27"/>
       <c r="W15" s="8"/>
       <c r="X15" s="8"/>
       <c r="Y15" s="8"/>
     </row>
     <row r="16" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="B16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
       <c r="V16" s="8"/>
       <c r="W16" s="8"/>
       <c r="X16" s="8"/>
       <c r="Y16" s="8"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="X17" s="2"/>
-      <c r="Y17" s="2"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -1190,28 +1196,28 @@
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
@@ -1219,27 +1225,27 @@
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+        <v>24</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
       <c r="V20" s="4"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
@@ -1248,27 +1254,27 @@
     <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="4"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="2"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
       <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="19"/>
       <c r="V21" s="4"/>
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
@@ -1277,28 +1283,28 @@
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
       <c r="S22" s="4"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="4"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
@@ -1306,73 +1312,73 @@
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
-      <c r="Q23" s="6"/>
+      <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="4"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="2"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="2"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
@@ -1393,15 +1399,15 @@
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="25"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
@@ -1422,19 +1428,19 @@
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="22"/>
       <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
@@ -1451,25 +1457,25 @@
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
@@ -1480,7 +1486,7 @@
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1489,12 +1495,12 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
@@ -1509,7 +1515,7 @@
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1519,13 +1525,13 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
@@ -1538,7 +1544,7 @@
     <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1549,26 +1555,26 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="6"/>
-      <c r="S31" s="6"/>
-      <c r="T31" s="6"/>
-      <c r="U31" s="6"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="12"/>
+      <c r="U31" s="12"/>
       <c r="V31" s="6"/>
       <c r="W31" s="6"/>
-      <c r="X31" s="2"/>
+      <c r="X31" s="19"/>
       <c r="Y31" s="2"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="2"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1584,35 +1590,35 @@
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
-      <c r="V32" s="2"/>
-      <c r="W32" s="2"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="13"/>
+      <c r="A33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
@@ -1625,23 +1631,23 @@
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="C34" s="12"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="6"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="6"/>
+      <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
@@ -1654,63 +1660,63 @@
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
-      <c r="T35" s="14"/>
-      <c r="U35" s="14"/>
-      <c r="V35" s="14"/>
-      <c r="W35" s="14"/>
-      <c r="X35" s="14"/>
-      <c r="Y35" s="14"/>
+        <v>16</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
-      <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
-      <c r="X36" s="2"/>
-      <c r="Y36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
+      <c r="W36" s="13"/>
+      <c r="X36" s="13"/>
+      <c r="Y36" s="13"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1737,27 +1743,27 @@
       <c r="Y37" s="2"/>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="6"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
@@ -1768,27 +1774,27 @@
     <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="12"/>
+      <c r="P39" s="12"/>
+      <c r="Q39" s="12"/>
+      <c r="R39" s="12"/>
+      <c r="S39" s="12"/>
+      <c r="T39" s="12"/>
+      <c r="U39" s="12"/>
       <c r="V39" s="2"/>
       <c r="W39" s="2"/>
       <c r="X39" s="2"/>
@@ -1797,23 +1803,23 @@
     <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="13"/>
-      <c r="P40" s="13"/>
-      <c r="Q40" s="13"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
@@ -1826,7 +1832,7 @@
     <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1839,12 +1845,12 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
-      <c r="Q41" s="13"/>
-      <c r="R41" s="13"/>
-      <c r="S41" s="13"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
@@ -1854,7 +1860,9 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
+      <c r="B42" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1869,9 +1877,9 @@
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4"/>
-      <c r="S42" s="4"/>
+      <c r="Q42" s="12"/>
+      <c r="R42" s="12"/>
+      <c r="S42" s="12"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
@@ -1880,9 +1888,7 @@
       <c r="Y42" s="2"/>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1898,9 +1904,9 @@
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
-      <c r="R43" s="2"/>
-      <c r="S43" s="2"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
@@ -1909,17 +1915,17 @@
       <c r="Y43" s="2"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
+      <c r="A44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
@@ -1927,9 +1933,9 @@
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="6"/>
-      <c r="S44" s="6"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
@@ -1940,67 +1946,96 @@
     <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
-      <c r="P45" s="15"/>
-      <c r="Q45" s="15"/>
-      <c r="R45" s="15"/>
-      <c r="S45" s="15"/>
-      <c r="T45" s="15"/>
-      <c r="U45" s="15"/>
-      <c r="V45" s="15"/>
-      <c r="W45" s="15"/>
-      <c r="X45" s="15"/>
-      <c r="Y45" s="15"/>
+        <v>22</v>
+      </c>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12"/>
+      <c r="S45" s="12"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+      <c r="X45" s="2"/>
+      <c r="Y45" s="2"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="R46" s="2"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
-      <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
-      <c r="W46" s="2"/>
-      <c r="X46" s="2"/>
-      <c r="Y46" s="2"/>
+      <c r="B46" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
+      <c r="N46" s="24"/>
+      <c r="O46" s="24"/>
+      <c r="P46" s="24"/>
+      <c r="Q46" s="24"/>
+      <c r="R46" s="24"/>
+      <c r="S46" s="24"/>
+      <c r="T46" s="24"/>
+      <c r="U46" s="24"/>
+      <c r="V46" s="14"/>
+      <c r="W46" s="14"/>
+      <c r="X46" s="14"/>
+      <c r="Y46" s="14"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+      <c r="X47" s="2"/>
+      <c r="Y47" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="W1:Y1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="R1:V1"/>
-    <mergeCell ref="W1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>